<commit_message>
Add create system user function
</commit_message>
<xml_diff>
--- a/role_permission_files/AdminPortal_Configuration_v0.40.xlsx
+++ b/role_permission_files/AdminPortal_Configuration_v0.40.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Product Management &amp; Market Research\Product Development\Platform\Admin Portal\AdminPortalRevamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\projects\sso_rws\role_permission_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="238">
   <si>
     <t>Version</t>
   </si>
@@ -804,6 +804,18 @@
   </si>
   <si>
     <t>add list change log for SSO</t>
+  </si>
+  <si>
+    <t>list_create_user_change_log</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>domain_casino_mapping</t>
+  </si>
+  <si>
+    <t>inactive</t>
   </si>
 </sst>
 </file>
@@ -1156,6 +1168,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1183,38 +1225,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2378,10 +2390,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="66"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="23" t="s">
         <v>8</v>
       </c>
@@ -2432,7 +2444,7 @@
       <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="57" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -2441,7 +2453,7 @@
       <c r="C5" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="60" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="22"/>
@@ -2458,14 +2470,14 @@
       <c r="J5" s="44"/>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-      <c r="B6" s="68" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="51" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="67"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="16" t="s">
         <v>10</v>
       </c>
@@ -2482,12 +2494,12 @@
       <c r="J6" s="44"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
-      <c r="B7" s="68"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="67"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="16"/>
       <c r="F7" s="22" t="s">
         <v>10</v>
@@ -2502,12 +2514,12 @@
       <c r="J7" s="44"/>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
-      <c r="B8" s="68"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="67"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="16"/>
       <c r="F8" s="22" t="s">
         <v>10</v>
@@ -2522,12 +2534,12 @@
       <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="68"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="67"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="18"/>
       <c r="F9" s="11" t="s">
         <v>10</v>
@@ -2542,12 +2554,12 @@
       <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="68"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="67"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="17"/>
       <c r="F10" s="11" t="s">
         <v>10</v>
@@ -2562,12 +2574,12 @@
       <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="68"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="67"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="18"/>
       <c r="F11" s="11" t="s">
         <v>10</v>
@@ -2582,14 +2594,14 @@
       <c r="J11" s="44"/>
     </row>
     <row r="12" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="68" t="s">
+      <c r="A12" s="58"/>
+      <c r="B12" s="51" t="s">
         <v>77</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="60" t="s">
         <v>77</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -2608,12 +2620,12 @@
       <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
-      <c r="B13" s="68"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="D13" s="67"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22" t="s">
         <v>10</v>
@@ -2628,12 +2640,12 @@
       <c r="J13" s="44"/>
     </row>
     <row r="14" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
-      <c r="B14" s="68"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="67"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
         <v>10</v>
@@ -2648,12 +2660,12 @@
       <c r="J14" s="44"/>
     </row>
     <row r="15" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="68"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="D15" s="67"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22" t="s">
         <v>10</v>
@@ -2668,12 +2680,12 @@
       <c r="J15" s="44"/>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
-      <c r="B16" s="68"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="D16" s="67"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="33"/>
       <c r="F16" s="33" t="s">
         <v>10</v>
@@ -2688,12 +2700,12 @@
       <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
-      <c r="B17" s="68"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="67"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22" t="s">
         <v>10</v>
@@ -2708,12 +2720,12 @@
       <c r="J17" s="44"/>
     </row>
     <row r="18" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="68"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="67"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22" t="s">
         <v>10</v>
@@ -2728,12 +2740,12 @@
       <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="68"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="67"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="19"/>
       <c r="F19" s="22" t="s">
         <v>10</v>
@@ -2748,12 +2760,12 @@
       <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D20" s="67"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="19"/>
       <c r="F20" s="22" t="s">
         <v>10</v>
@@ -2768,12 +2780,12 @@
       <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
-      <c r="B21" s="68"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="67"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22" t="s">
         <v>10</v>
@@ -2786,12 +2798,12 @@
       <c r="J21" s="44"/>
     </row>
     <row r="22" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
-      <c r="B22" s="68"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="67"/>
+      <c r="D22" s="60"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22" t="s">
         <v>10</v>
@@ -2804,14 +2816,14 @@
       <c r="J22" s="44"/>
     </row>
     <row r="23" spans="1:10" s="9" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
-      <c r="B23" s="60" t="s">
+      <c r="A23" s="58"/>
+      <c r="B23" s="57" t="s">
         <v>111</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="54" t="s">
         <v>145</v>
       </c>
       <c r="E23" s="28" t="s">
@@ -2832,12 +2844,12 @@
       <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" s="9" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="64"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="40" t="s">
         <v>10</v>
       </c>
@@ -2852,12 +2864,12 @@
       <c r="J24" s="44"/>
     </row>
     <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="61"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="64"/>
+      <c r="D25" s="55"/>
       <c r="E25" s="40" t="s">
         <v>10</v>
       </c>
@@ -2876,12 +2888,12 @@
       <c r="J25" s="44"/>
     </row>
     <row r="26" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="62"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="65"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="40"/>
       <c r="F26" s="40" t="s">
         <v>10</v>
@@ -2894,16 +2906,16 @@
       <c r="J26" s="44"/>
     </row>
     <row r="27" spans="1:10" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="51" t="s">
         <v>97</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="67" t="s">
+      <c r="D27" s="60" t="s">
         <v>98</v>
       </c>
       <c r="E27" s="22"/>
@@ -2922,12 +2934,12 @@
       <c r="J27" s="44"/>
     </row>
     <row r="28" spans="1:10" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
-      <c r="B28" s="68"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="D28" s="67"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22" t="s">
         <v>10</v>
@@ -2942,12 +2954,12 @@
       <c r="J28" s="44"/>
     </row>
     <row r="29" spans="1:10" s="9" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
-      <c r="B29" s="68"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="67"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22" t="s">
         <v>10</v>
@@ -2962,7 +2974,7 @@
       <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="58"/>
       <c r="B30" s="21" t="s">
         <v>99</v>
       </c>
@@ -2990,14 +3002,14 @@
       <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" s="9" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
-      <c r="B31" s="68" t="s">
+      <c r="A31" s="58"/>
+      <c r="B31" s="51" t="s">
         <v>101</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D31" s="67" t="s">
+      <c r="D31" s="60" t="s">
         <v>193</v>
       </c>
       <c r="E31" s="22"/>
@@ -3010,12 +3022,12 @@
       <c r="J31" s="44"/>
     </row>
     <row r="32" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
-      <c r="B32" s="68"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="67"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -3026,7 +3038,7 @@
       <c r="J32" s="44"/>
     </row>
     <row r="33" spans="1:10" s="9" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="58"/>
       <c r="B33" s="36" t="s">
         <v>130</v>
       </c>
@@ -3054,110 +3066,110 @@
       <c r="J33" s="44"/>
     </row>
     <row r="34" spans="1:10" s="9" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="63" t="s">
+      <c r="D34" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="53"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="63"/>
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
-      <c r="B35" s="60" t="s">
+      <c r="A35" s="58"/>
+      <c r="B35" s="57" t="s">
         <v>56</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="56"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="66"/>
     </row>
     <row r="36" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="61"/>
-      <c r="B36" s="61"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
       <c r="C36" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="56"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="66"/>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
-      <c r="B37" s="61"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="56"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="66"/>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
-      <c r="B38" s="61"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="58"/>
       <c r="C38" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="56"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="66"/>
     </row>
     <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="61"/>
-      <c r="B39" s="61"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="56"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="66"/>
     </row>
     <row r="40" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
-      <c r="B40" s="62"/>
+      <c r="A40" s="59"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="65"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="59"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="69"/>
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" ht="129" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -3186,16 +3198,16 @@
       <c r="J41" s="44"/>
     </row>
     <row r="42" spans="1:10" s="9" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="69" t="s">
+      <c r="A42" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="51" t="s">
         <v>134</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="63" t="s">
+      <c r="D42" s="54" t="s">
         <v>135</v>
       </c>
       <c r="E42" s="39" t="s">
@@ -3216,12 +3228,12 @@
       <c r="J42" s="44"/>
     </row>
     <row r="43" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="70"/>
-      <c r="B43" s="68"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="64"/>
+      <c r="D43" s="55"/>
       <c r="E43" s="39" t="s">
         <v>10</v>
       </c>
@@ -3236,12 +3248,12 @@
       <c r="J43" s="44"/>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
-      <c r="B44" s="68"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="64"/>
+      <c r="D44" s="55"/>
       <c r="E44" s="39" t="s">
         <v>10</v>
       </c>
@@ -3256,12 +3268,12 @@
       <c r="J44" s="44"/>
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="70"/>
-      <c r="B45" s="68"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="D45" s="64"/>
+      <c r="D45" s="55"/>
       <c r="E45" s="39" t="s">
         <v>10</v>
       </c>
@@ -3276,12 +3288,12 @@
       <c r="J45" s="44"/>
     </row>
     <row r="46" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
-      <c r="B46" s="68"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="64"/>
+      <c r="D46" s="55"/>
       <c r="E46" s="39" t="s">
         <v>10</v>
       </c>
@@ -3298,12 +3310,12 @@
       <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="70"/>
-      <c r="B47" s="68"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="64"/>
+      <c r="D47" s="55"/>
       <c r="E47" s="39" t="s">
         <v>10</v>
       </c>
@@ -3322,12 +3334,12 @@
       <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="70"/>
-      <c r="B48" s="68"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="D48" s="64"/>
+      <c r="D48" s="55"/>
       <c r="E48" s="39" t="s">
         <v>10</v>
       </c>
@@ -3344,12 +3356,12 @@
       <c r="J48" s="44"/>
     </row>
     <row r="49" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="70"/>
-      <c r="B49" s="68"/>
+      <c r="A49" s="53"/>
+      <c r="B49" s="51"/>
       <c r="C49" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="D49" s="64"/>
+      <c r="D49" s="55"/>
       <c r="E49" s="39" t="s">
         <v>10</v>
       </c>
@@ -3364,12 +3376,12 @@
       <c r="J49" s="44"/>
     </row>
     <row r="50" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="70"/>
-      <c r="B50" s="68"/>
+      <c r="A50" s="53"/>
+      <c r="B50" s="51"/>
       <c r="C50" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="D50" s="64"/>
+      <c r="D50" s="55"/>
       <c r="E50" s="39" t="s">
         <v>10</v>
       </c>
@@ -3386,12 +3398,12 @@
       <c r="J50" s="44"/>
     </row>
     <row r="51" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="70"/>
-      <c r="B51" s="68"/>
+      <c r="A51" s="53"/>
+      <c r="B51" s="51"/>
       <c r="C51" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="65"/>
+      <c r="D51" s="56"/>
       <c r="E51" s="39"/>
       <c r="F51" s="39" t="s">
         <v>10</v>
@@ -3419,6 +3431,15 @@
     <row r="65" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E34:J40"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A5:A26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D5:D11"/>
+    <mergeCell ref="D12:D22"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B22"/>
     <mergeCell ref="B42:B51"/>
     <mergeCell ref="A42:A51"/>
     <mergeCell ref="D42:D51"/>
@@ -3429,15 +3450,6 @@
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D34:D40"/>
     <mergeCell ref="B35:B40"/>
-    <mergeCell ref="E34:J40"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A5:A26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D5:D11"/>
-    <mergeCell ref="D12:D22"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6833,10 +6845,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="66"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="27" t="s">
         <v>8</v>
       </c>
@@ -6854,16 +6866,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="54" t="s">
         <v>55</v>
       </c>
       <c r="E4" s="49" t="s">
@@ -6880,12 +6892,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="61"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="64"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="49" t="s">
         <v>10</v>
       </c>
@@ -6897,12 +6909,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="49" t="s">
         <v>10</v>
       </c>
@@ -6937,10 +6949,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="51" t="s">
         <v>114</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -6960,8 +6972,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="68"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="16" t="s">
         <v>131</v>
       </c>
@@ -6983,12 +6995,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D4:D6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6997,9 +7009,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7200,16 +7214,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>192</v>
@@ -7238,16 +7252,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>192</v>
@@ -7276,80 +7290,95 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>191</v>
+      <c r="C10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>191</v>
@@ -7357,22 +7386,37 @@
       <c r="G10" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>191</v>
+      <c r="A11" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>191</v>
@@ -7380,22 +7424,25 @@
       <c r="G11" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>191</v>
+      <c r="A12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>191</v>
@@ -7403,22 +7450,25 @@
       <c r="G12" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>191</v>
+      <c r="A13" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>191</v>
@@ -7426,22 +7476,25 @@
       <c r="G13" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>191</v>
+      <c r="A14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>191</v>
@@ -7449,22 +7502,25 @@
       <c r="G14" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>191</v>
+      <c r="A15" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>191</v>
@@ -7472,28 +7528,37 @@
       <c r="G15" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>191</v>
+      <c r="A16" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>191</v>
       </c>
@@ -7512,8 +7577,11 @@
       <c r="F17" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>191</v>
       </c>
@@ -7533,7 +7601,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>191</v>
       </c>
@@ -7553,7 +7621,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>191</v>
       </c>
@@ -7573,7 +7641,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>191</v>
       </c>
@@ -7593,7 +7661,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>191</v>
       </c>
@@ -7613,7 +7681,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>191</v>
       </c>
@@ -7633,7 +7701,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>191</v>
       </c>
@@ -7653,7 +7721,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>191</v>
       </c>
@@ -7673,7 +7741,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>191</v>
       </c>
@@ -7690,6 +7758,46 @@
         <v>191</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>